<commit_message>
update to all integration tests
</commit_message>
<xml_diff>
--- a/IntegrationStrategy.xlsx
+++ b/IntegrationStrategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\4. Sem\SWT\SWT_Assignment3_GR16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9A1D97-A3E0-4101-A320-99842DBE8697}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE2DF5A-EAAD-4B99-890F-C0A31CCF88E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{9CBD800E-6A27-47EA-B1F7-BFA7CE6A41AB}"/>
   </bookViews>
@@ -231,14 +231,14 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,7 +563,7 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
   <sheetData>
     <row r="1" spans="2:12" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -611,7 +611,7 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="7">
         <v>1</v>
       </c>
@@ -636,7 +636,7 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="8">
         <v>2</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7">
         <v>3</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="L5" s="5"/>
     </row>
     <row r="6" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="8">
         <f>C5+1</f>
         <v>4</v>
@@ -710,7 +710,7 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7">
         <f t="shared" ref="C7:C13" si="0">C6+1</f>
         <v>5</v>
@@ -734,7 +734,7 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -750,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -762,7 +762,7 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -788,13 +788,15 @@
       <c r="J9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="5"/>
+      <c r="K9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -803,30 +805,28 @@
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="12" t="s">
+      <c r="K10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:12" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -836,7 +836,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="H11" s="5"/>
@@ -846,7 +846,7 @@
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="6"/>
@@ -866,7 +866,7 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -874,7 +874,7 @@
       <c r="D13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="5"/>

</xml_diff>